<commit_message>
Minor updates for user experience
</commit_message>
<xml_diff>
--- a/Data/Redraft_Matchups.xlsx
+++ b/Data/Redraft_Matchups.xlsx
@@ -83924,7 +83924,7 @@
         <v>689</v>
       </c>
       <c r="G3564">
-        <v>2.8</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="3565" spans="2:7">
@@ -84664,7 +84664,7 @@
         <v>689</v>
       </c>
       <c r="G3601">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3602" spans="2:7">
@@ -86744,7 +86744,7 @@
         <v>689</v>
       </c>
       <c r="G3705">
-        <v>10.44</v>
+        <v>10.88</v>
       </c>
     </row>
     <row r="3706" spans="2:7">

</xml_diff>

<commit_message>
Initial Demo and Flask building
</commit_message>
<xml_diff>
--- a/Data/Redraft_Matchups.xlsx
+++ b/Data/Redraft_Matchups.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14972" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14968" uniqueCount="692">
   <si>
     <t>week</t>
   </si>
@@ -2447,7 +2447,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H3742"/>
+  <dimension ref="A1:H3741"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -94159,7 +94159,7 @@
         <v>690</v>
       </c>
       <c r="H3544">
-        <v>0</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="3545" spans="1:8">
@@ -94297,7 +94297,7 @@
         <v>690</v>
       </c>
       <c r="H3550">
-        <v>0</v>
+        <v>31.8</v>
       </c>
     </row>
     <row r="3551" spans="1:8">
@@ -94320,7 +94320,7 @@
         <v>691</v>
       </c>
       <c r="H3551">
-        <v>5</v>
+        <v>16.1</v>
       </c>
     </row>
     <row r="3552" spans="1:8">
@@ -94412,7 +94412,7 @@
         <v>691</v>
       </c>
       <c r="H3555">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3556" spans="1:8">
@@ -94435,7 +94435,7 @@
         <v>691</v>
       </c>
       <c r="H3556">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3557" spans="1:8">
@@ -94573,7 +94573,7 @@
         <v>690</v>
       </c>
       <c r="H3562">
-        <v>0</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="3563" spans="1:8">
@@ -94619,7 +94619,7 @@
         <v>690</v>
       </c>
       <c r="H3564">
-        <v>6.3</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="3565" spans="1:8">
@@ -94665,7 +94665,7 @@
         <v>690</v>
       </c>
       <c r="H3566">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="3567" spans="1:8">
@@ -94826,7 +94826,7 @@
         <v>690</v>
       </c>
       <c r="H3573">
-        <v>0</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="3574" spans="1:8">
@@ -94863,13 +94863,13 @@
         <v>10</v>
       </c>
       <c r="E3575" t="s">
-        <v>351</v>
+        <v>57</v>
       </c>
       <c r="F3575" t="s">
-        <v>686</v>
+        <v>392</v>
       </c>
       <c r="G3575" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3575">
         <v>0</v>
@@ -94886,16 +94886,16 @@
         <v>10</v>
       </c>
       <c r="E3576" t="s">
-        <v>352</v>
+        <v>59</v>
       </c>
       <c r="F3576" t="s">
-        <v>687</v>
+        <v>394</v>
       </c>
       <c r="G3576" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3576">
-        <v>0</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="3577" spans="1:8">
@@ -94909,16 +94909,16 @@
         <v>10</v>
       </c>
       <c r="E3577" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="F3577" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="G3577" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3577">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="3578" spans="1:8">
@@ -94932,10 +94932,10 @@
         <v>10</v>
       </c>
       <c r="E3578" t="s">
-        <v>59</v>
+        <v>251</v>
       </c>
       <c r="F3578" t="s">
-        <v>394</v>
+        <v>586</v>
       </c>
       <c r="G3578" t="s">
         <v>690</v>
@@ -94955,13 +94955,13 @@
         <v>10</v>
       </c>
       <c r="E3579" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F3579" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="G3579" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3579">
         <v>0</v>
@@ -94978,13 +94978,13 @@
         <v>10</v>
       </c>
       <c r="E3580" t="s">
-        <v>251</v>
+        <v>194</v>
       </c>
       <c r="F3580" t="s">
-        <v>586</v>
+        <v>529</v>
       </c>
       <c r="G3580" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3580">
         <v>0</v>
@@ -95001,13 +95001,13 @@
         <v>10</v>
       </c>
       <c r="E3581" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F3581" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="G3581" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3581">
         <v>0</v>
@@ -95024,13 +95024,13 @@
         <v>10</v>
       </c>
       <c r="E3582" t="s">
-        <v>194</v>
+        <v>173</v>
       </c>
       <c r="F3582" t="s">
-        <v>529</v>
+        <v>508</v>
       </c>
       <c r="G3582" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3582">
         <v>0</v>
@@ -95047,10 +95047,10 @@
         <v>10</v>
       </c>
       <c r="E3583" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F3583" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="G3583" t="s">
         <v>691</v>
@@ -95070,10 +95070,10 @@
         <v>10</v>
       </c>
       <c r="E3584" t="s">
-        <v>173</v>
+        <v>66</v>
       </c>
       <c r="F3584" t="s">
-        <v>508</v>
+        <v>401</v>
       </c>
       <c r="G3584" t="s">
         <v>690</v>
@@ -95093,13 +95093,13 @@
         <v>10</v>
       </c>
       <c r="E3585" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F3585" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="G3585" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3585">
         <v>0</v>
@@ -95116,16 +95116,16 @@
         <v>10</v>
       </c>
       <c r="E3586" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F3586" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="G3586" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3586">
-        <v>0</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="3587" spans="1:8">
@@ -95139,13 +95139,13 @@
         <v>10</v>
       </c>
       <c r="E3587" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="F3587" t="s">
-        <v>404</v>
+        <v>517</v>
       </c>
       <c r="G3587" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3587">
         <v>0</v>
@@ -95156,19 +95156,19 @@
         <v>18</v>
       </c>
       <c r="C3588">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D3588" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3588" t="s">
-        <v>182</v>
+        <v>302</v>
       </c>
       <c r="F3588" t="s">
-        <v>517</v>
+        <v>637</v>
       </c>
       <c r="G3588" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3588">
         <v>0</v>
@@ -95185,13 +95185,13 @@
         <v>11</v>
       </c>
       <c r="E3589" t="s">
-        <v>302</v>
+        <v>318</v>
       </c>
       <c r="F3589" t="s">
-        <v>637</v>
+        <v>653</v>
       </c>
       <c r="G3589" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3589">
         <v>0</v>
@@ -95208,16 +95208,16 @@
         <v>11</v>
       </c>
       <c r="E3590" t="s">
-        <v>318</v>
+        <v>74</v>
       </c>
       <c r="F3590" t="s">
-        <v>653</v>
+        <v>409</v>
       </c>
       <c r="G3590" t="s">
         <v>691</v>
       </c>
       <c r="H3590">
-        <v>0</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="3591" spans="1:8">
@@ -95231,10 +95231,10 @@
         <v>11</v>
       </c>
       <c r="E3591" t="s">
-        <v>74</v>
+        <v>244</v>
       </c>
       <c r="F3591" t="s">
-        <v>409</v>
+        <v>579</v>
       </c>
       <c r="G3591" t="s">
         <v>691</v>
@@ -95254,13 +95254,13 @@
         <v>11</v>
       </c>
       <c r="E3592" t="s">
-        <v>244</v>
+        <v>75</v>
       </c>
       <c r="F3592" t="s">
-        <v>579</v>
+        <v>410</v>
       </c>
       <c r="G3592" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3592">
         <v>0</v>
@@ -95277,10 +95277,10 @@
         <v>11</v>
       </c>
       <c r="E3593" t="s">
-        <v>75</v>
+        <v>91</v>
       </c>
       <c r="F3593" t="s">
-        <v>410</v>
+        <v>426</v>
       </c>
       <c r="G3593" t="s">
         <v>690</v>
@@ -95300,10 +95300,10 @@
         <v>11</v>
       </c>
       <c r="E3594" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="F3594" t="s">
-        <v>426</v>
+        <v>412</v>
       </c>
       <c r="G3594" t="s">
         <v>690</v>
@@ -95323,13 +95323,13 @@
         <v>11</v>
       </c>
       <c r="E3595" t="s">
-        <v>77</v>
+        <v>254</v>
       </c>
       <c r="F3595" t="s">
-        <v>412</v>
+        <v>589</v>
       </c>
       <c r="G3595" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3595">
         <v>0</v>
@@ -95346,16 +95346,16 @@
         <v>11</v>
       </c>
       <c r="E3596" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="F3596" t="s">
-        <v>589</v>
+        <v>604</v>
       </c>
       <c r="G3596" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3596">
-        <v>0</v>
+        <v>11.2</v>
       </c>
     </row>
     <row r="3597" spans="1:8">
@@ -95369,13 +95369,13 @@
         <v>11</v>
       </c>
       <c r="E3597" t="s">
-        <v>269</v>
+        <v>78</v>
       </c>
       <c r="F3597" t="s">
-        <v>604</v>
+        <v>413</v>
       </c>
       <c r="G3597" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3597">
         <v>0</v>
@@ -95392,13 +95392,13 @@
         <v>11</v>
       </c>
       <c r="E3598" t="s">
-        <v>78</v>
+        <v>223</v>
       </c>
       <c r="F3598" t="s">
-        <v>413</v>
+        <v>558</v>
       </c>
       <c r="G3598" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3598">
         <v>0</v>
@@ -95415,13 +95415,13 @@
         <v>11</v>
       </c>
       <c r="E3599" t="s">
-        <v>223</v>
+        <v>29</v>
       </c>
       <c r="F3599" t="s">
-        <v>558</v>
+        <v>364</v>
       </c>
       <c r="G3599" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3599">
         <v>0</v>
@@ -95438,16 +95438,16 @@
         <v>11</v>
       </c>
       <c r="E3600" t="s">
-        <v>29</v>
+        <v>80</v>
       </c>
       <c r="F3600" t="s">
-        <v>364</v>
+        <v>415</v>
       </c>
       <c r="G3600" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3600">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3601" spans="1:8">
@@ -95461,16 +95461,16 @@
         <v>11</v>
       </c>
       <c r="E3601" t="s">
-        <v>80</v>
+        <v>115</v>
       </c>
       <c r="F3601" t="s">
-        <v>415</v>
+        <v>450</v>
       </c>
       <c r="G3601" t="s">
         <v>690</v>
       </c>
       <c r="H3601">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3602" spans="1:8">
@@ -95484,16 +95484,16 @@
         <v>11</v>
       </c>
       <c r="E3602" t="s">
-        <v>115</v>
+        <v>81</v>
       </c>
       <c r="F3602" t="s">
-        <v>450</v>
+        <v>416</v>
       </c>
       <c r="G3602" t="s">
         <v>690</v>
       </c>
       <c r="H3602">
-        <v>0</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="3603" spans="1:8">
@@ -95507,13 +95507,13 @@
         <v>11</v>
       </c>
       <c r="E3603" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F3603" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="G3603" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3603">
         <v>0</v>
@@ -95530,10 +95530,10 @@
         <v>11</v>
       </c>
       <c r="E3604" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F3604" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="G3604" t="s">
         <v>691</v>
@@ -95553,10 +95553,10 @@
         <v>11</v>
       </c>
       <c r="E3605" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F3605" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="G3605" t="s">
         <v>691</v>
@@ -95576,10 +95576,10 @@
         <v>11</v>
       </c>
       <c r="E3606" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F3606" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="G3606" t="s">
         <v>691</v>
@@ -95593,22 +95593,22 @@
         <v>18</v>
       </c>
       <c r="C3607">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D3607" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3607" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="F3607" t="s">
-        <v>420</v>
+        <v>503</v>
       </c>
       <c r="G3607" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3607">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3608" spans="1:8">
@@ -95622,10 +95622,10 @@
         <v>12</v>
       </c>
       <c r="E3608" t="s">
-        <v>168</v>
+        <v>305</v>
       </c>
       <c r="F3608" t="s">
-        <v>503</v>
+        <v>640</v>
       </c>
       <c r="G3608" t="s">
         <v>690</v>
@@ -95645,10 +95645,10 @@
         <v>12</v>
       </c>
       <c r="E3609" t="s">
-        <v>305</v>
+        <v>226</v>
       </c>
       <c r="F3609" t="s">
-        <v>640</v>
+        <v>561</v>
       </c>
       <c r="G3609" t="s">
         <v>690</v>
@@ -95668,10 +95668,10 @@
         <v>12</v>
       </c>
       <c r="E3610" t="s">
-        <v>226</v>
+        <v>89</v>
       </c>
       <c r="F3610" t="s">
-        <v>561</v>
+        <v>424</v>
       </c>
       <c r="G3610" t="s">
         <v>690</v>
@@ -95691,13 +95691,13 @@
         <v>12</v>
       </c>
       <c r="E3611" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F3611" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="G3611" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3611">
         <v>0</v>
@@ -95714,10 +95714,10 @@
         <v>12</v>
       </c>
       <c r="E3612" t="s">
-        <v>90</v>
+        <v>353</v>
       </c>
       <c r="F3612" t="s">
-        <v>425</v>
+        <v>688</v>
       </c>
       <c r="G3612" t="s">
         <v>691</v>
@@ -95737,10 +95737,10 @@
         <v>12</v>
       </c>
       <c r="E3613" t="s">
-        <v>353</v>
+        <v>92</v>
       </c>
       <c r="F3613" t="s">
-        <v>688</v>
+        <v>427</v>
       </c>
       <c r="G3613" t="s">
         <v>691</v>
@@ -95760,13 +95760,13 @@
         <v>12</v>
       </c>
       <c r="E3614" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F3614" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="G3614" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3614">
         <v>0</v>
@@ -95783,13 +95783,13 @@
         <v>12</v>
       </c>
       <c r="E3615" t="s">
-        <v>93</v>
+        <v>62</v>
       </c>
       <c r="F3615" t="s">
-        <v>428</v>
+        <v>397</v>
       </c>
       <c r="G3615" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3615">
         <v>0</v>
@@ -95806,13 +95806,13 @@
         <v>12</v>
       </c>
       <c r="E3616" t="s">
-        <v>62</v>
+        <v>274</v>
       </c>
       <c r="F3616" t="s">
-        <v>397</v>
+        <v>609</v>
       </c>
       <c r="G3616" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3616">
         <v>0</v>
@@ -95829,16 +95829,16 @@
         <v>12</v>
       </c>
       <c r="E3617" t="s">
-        <v>274</v>
+        <v>354</v>
       </c>
       <c r="F3617" t="s">
-        <v>609</v>
+        <v>689</v>
       </c>
       <c r="G3617" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3617">
-        <v>0</v>
+        <v>2.7</v>
       </c>
     </row>
     <row r="3618" spans="1:8">
@@ -95852,13 +95852,13 @@
         <v>12</v>
       </c>
       <c r="E3618" t="s">
-        <v>354</v>
+        <v>176</v>
       </c>
       <c r="F3618" t="s">
-        <v>689</v>
+        <v>511</v>
       </c>
       <c r="G3618" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3618">
         <v>0</v>
@@ -95875,10 +95875,10 @@
         <v>12</v>
       </c>
       <c r="E3619" t="s">
-        <v>176</v>
+        <v>95</v>
       </c>
       <c r="F3619" t="s">
-        <v>511</v>
+        <v>430</v>
       </c>
       <c r="G3619" t="s">
         <v>690</v>
@@ -95898,13 +95898,13 @@
         <v>12</v>
       </c>
       <c r="E3620" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F3620" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="G3620" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3620">
         <v>0</v>
@@ -95921,10 +95921,10 @@
         <v>12</v>
       </c>
       <c r="E3621" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F3621" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="G3621" t="s">
         <v>691</v>
@@ -95944,13 +95944,13 @@
         <v>12</v>
       </c>
       <c r="E3622" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F3622" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="G3622" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3622">
         <v>0</v>
@@ -95967,16 +95967,16 @@
         <v>12</v>
       </c>
       <c r="E3623" t="s">
-        <v>99</v>
+        <v>339</v>
       </c>
       <c r="F3623" t="s">
-        <v>434</v>
+        <v>674</v>
       </c>
       <c r="G3623" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3623">
-        <v>0</v>
+        <v>2.3</v>
       </c>
     </row>
     <row r="3624" spans="1:8">
@@ -95990,10 +95990,10 @@
         <v>12</v>
       </c>
       <c r="E3624" t="s">
-        <v>339</v>
+        <v>200</v>
       </c>
       <c r="F3624" t="s">
-        <v>674</v>
+        <v>535</v>
       </c>
       <c r="G3624" t="s">
         <v>691</v>
@@ -96007,19 +96007,19 @@
         <v>18</v>
       </c>
       <c r="C3625">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3625" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3625" t="s">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="F3625" t="s">
-        <v>535</v>
+        <v>575</v>
       </c>
       <c r="G3625" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3625">
         <v>0</v>
@@ -96036,10 +96036,10 @@
         <v>13</v>
       </c>
       <c r="E3626" t="s">
-        <v>240</v>
+        <v>310</v>
       </c>
       <c r="F3626" t="s">
-        <v>575</v>
+        <v>645</v>
       </c>
       <c r="G3626" t="s">
         <v>690</v>
@@ -96059,16 +96059,16 @@
         <v>13</v>
       </c>
       <c r="E3627" t="s">
-        <v>310</v>
+        <v>104</v>
       </c>
       <c r="F3627" t="s">
-        <v>645</v>
+        <v>439</v>
       </c>
       <c r="G3627" t="s">
         <v>690</v>
       </c>
       <c r="H3627">
-        <v>0</v>
+        <v>3.6</v>
       </c>
     </row>
     <row r="3628" spans="1:8">
@@ -96082,10 +96082,10 @@
         <v>13</v>
       </c>
       <c r="E3628" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="F3628" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="G3628" t="s">
         <v>690</v>
@@ -96105,13 +96105,13 @@
         <v>13</v>
       </c>
       <c r="E3629" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="F3629" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="G3629" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3629">
         <v>0</v>
@@ -96128,10 +96128,10 @@
         <v>13</v>
       </c>
       <c r="E3630" t="s">
-        <v>106</v>
+        <v>313</v>
       </c>
       <c r="F3630" t="s">
-        <v>441</v>
+        <v>648</v>
       </c>
       <c r="G3630" t="s">
         <v>691</v>
@@ -96151,13 +96151,13 @@
         <v>13</v>
       </c>
       <c r="E3631" t="s">
-        <v>313</v>
+        <v>193</v>
       </c>
       <c r="F3631" t="s">
-        <v>648</v>
+        <v>528</v>
       </c>
       <c r="G3631" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3631">
         <v>0</v>
@@ -96174,13 +96174,13 @@
         <v>13</v>
       </c>
       <c r="E3632" t="s">
-        <v>193</v>
+        <v>263</v>
       </c>
       <c r="F3632" t="s">
-        <v>528</v>
+        <v>598</v>
       </c>
       <c r="G3632" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3632">
         <v>0</v>
@@ -96197,13 +96197,13 @@
         <v>13</v>
       </c>
       <c r="E3633" t="s">
-        <v>263</v>
+        <v>108</v>
       </c>
       <c r="F3633" t="s">
-        <v>598</v>
+        <v>443</v>
       </c>
       <c r="G3633" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3633">
         <v>0</v>
@@ -96220,13 +96220,13 @@
         <v>13</v>
       </c>
       <c r="E3634" t="s">
-        <v>108</v>
+        <v>268</v>
       </c>
       <c r="F3634" t="s">
-        <v>443</v>
+        <v>603</v>
       </c>
       <c r="G3634" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3634">
         <v>0</v>
@@ -96243,13 +96243,13 @@
         <v>13</v>
       </c>
       <c r="E3635" t="s">
-        <v>268</v>
+        <v>111</v>
       </c>
       <c r="F3635" t="s">
-        <v>603</v>
+        <v>446</v>
       </c>
       <c r="G3635" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3635">
         <v>0</v>
@@ -96266,13 +96266,13 @@
         <v>13</v>
       </c>
       <c r="E3636" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F3636" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="G3636" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3636">
         <v>0</v>
@@ -96289,13 +96289,13 @@
         <v>13</v>
       </c>
       <c r="E3637" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F3637" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="G3637" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3637">
         <v>0</v>
@@ -96312,13 +96312,13 @@
         <v>13</v>
       </c>
       <c r="E3638" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F3638" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="G3638" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3638">
         <v>0</v>
@@ -96335,16 +96335,16 @@
         <v>13</v>
       </c>
       <c r="E3639" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F3639" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="G3639" t="s">
         <v>691</v>
       </c>
       <c r="H3639">
-        <v>0</v>
+        <v>11.4</v>
       </c>
     </row>
     <row r="3640" spans="1:8">
@@ -96358,16 +96358,16 @@
         <v>13</v>
       </c>
       <c r="E3640" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="F3640" t="s">
-        <v>452</v>
+        <v>421</v>
       </c>
       <c r="G3640" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3640">
-        <v>8.199999999999999</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3641" spans="1:8">
@@ -96375,16 +96375,16 @@
         <v>18</v>
       </c>
       <c r="C3641">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3641" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E3641" t="s">
-        <v>86</v>
+        <v>152</v>
       </c>
       <c r="F3641" t="s">
-        <v>421</v>
+        <v>487</v>
       </c>
       <c r="G3641" t="s">
         <v>690</v>
@@ -96404,13 +96404,13 @@
         <v>14</v>
       </c>
       <c r="E3642" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="F3642" t="s">
-        <v>487</v>
+        <v>454</v>
       </c>
       <c r="G3642" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3642">
         <v>0</v>
@@ -96427,10 +96427,10 @@
         <v>14</v>
       </c>
       <c r="E3643" t="s">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="F3643" t="s">
-        <v>454</v>
+        <v>390</v>
       </c>
       <c r="G3643" t="s">
         <v>691</v>
@@ -96450,13 +96450,13 @@
         <v>14</v>
       </c>
       <c r="E3644" t="s">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="F3644" t="s">
-        <v>390</v>
+        <v>455</v>
       </c>
       <c r="G3644" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3644">
         <v>0</v>
@@ -96473,16 +96473,16 @@
         <v>14</v>
       </c>
       <c r="E3645" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F3645" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="G3645" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3645">
-        <v>0</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="3646" spans="1:8">
@@ -96496,13 +96496,13 @@
         <v>14</v>
       </c>
       <c r="E3646" t="s">
-        <v>121</v>
+        <v>241</v>
       </c>
       <c r="F3646" t="s">
-        <v>456</v>
+        <v>576</v>
       </c>
       <c r="G3646" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3646">
         <v>0</v>
@@ -96519,10 +96519,10 @@
         <v>14</v>
       </c>
       <c r="E3647" t="s">
-        <v>241</v>
+        <v>123</v>
       </c>
       <c r="F3647" t="s">
-        <v>576</v>
+        <v>458</v>
       </c>
       <c r="G3647" t="s">
         <v>690</v>
@@ -96542,10 +96542,10 @@
         <v>14</v>
       </c>
       <c r="E3648" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F3648" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="G3648" t="s">
         <v>690</v>
@@ -96565,13 +96565,13 @@
         <v>14</v>
       </c>
       <c r="E3649" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="F3649" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="G3649" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3649">
         <v>0</v>
@@ -96588,13 +96588,13 @@
         <v>14</v>
       </c>
       <c r="E3650" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="F3650" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="G3650" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3650">
         <v>0</v>
@@ -96611,16 +96611,16 @@
         <v>14</v>
       </c>
       <c r="E3651" t="s">
-        <v>128</v>
+        <v>224</v>
       </c>
       <c r="F3651" t="s">
-        <v>463</v>
+        <v>559</v>
       </c>
       <c r="G3651" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3651">
-        <v>0</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="3652" spans="1:8">
@@ -96634,16 +96634,16 @@
         <v>14</v>
       </c>
       <c r="E3652" t="s">
-        <v>224</v>
+        <v>129</v>
       </c>
       <c r="F3652" t="s">
-        <v>559</v>
+        <v>464</v>
       </c>
       <c r="G3652" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3652">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3653" spans="1:8">
@@ -96657,16 +96657,16 @@
         <v>14</v>
       </c>
       <c r="E3653" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="F3653" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="G3653" t="s">
         <v>690</v>
       </c>
       <c r="H3653">
-        <v>0</v>
+        <v>10.4</v>
       </c>
     </row>
     <row r="3654" spans="1:8">
@@ -96680,13 +96680,13 @@
         <v>14</v>
       </c>
       <c r="E3654" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F3654" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="G3654" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3654">
         <v>0</v>
@@ -96703,10 +96703,10 @@
         <v>14</v>
       </c>
       <c r="E3655" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F3655" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="G3655" t="s">
         <v>691</v>
@@ -96726,13 +96726,13 @@
         <v>14</v>
       </c>
       <c r="E3656" t="s">
-        <v>133</v>
+        <v>291</v>
       </c>
       <c r="F3656" t="s">
-        <v>468</v>
+        <v>626</v>
       </c>
       <c r="G3656" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3656">
         <v>0</v>
@@ -96749,13 +96749,13 @@
         <v>14</v>
       </c>
       <c r="E3657" t="s">
-        <v>291</v>
+        <v>134</v>
       </c>
       <c r="F3657" t="s">
-        <v>626</v>
+        <v>469</v>
       </c>
       <c r="G3657" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3657">
         <v>0</v>
@@ -96766,19 +96766,19 @@
         <v>18</v>
       </c>
       <c r="C3658">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3658" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3658" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="F3658" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="G3658" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3658">
         <v>0</v>
@@ -96795,16 +96795,16 @@
         <v>15</v>
       </c>
       <c r="E3659" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F3659" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="G3659" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3659">
-        <v>0</v>
+        <v>6.94</v>
       </c>
     </row>
     <row r="3660" spans="1:8">
@@ -96818,16 +96818,16 @@
         <v>15</v>
       </c>
       <c r="E3660" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F3660" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="G3660" t="s">
         <v>691</v>
       </c>
       <c r="H3660">
-        <v>0</v>
+        <v>5.6</v>
       </c>
     </row>
     <row r="3661" spans="1:8">
@@ -96841,16 +96841,16 @@
         <v>15</v>
       </c>
       <c r="E3661" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F3661" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="G3661" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3661">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3662" spans="1:8">
@@ -96864,13 +96864,13 @@
         <v>15</v>
       </c>
       <c r="E3662" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F3662" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="G3662" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3662">
         <v>0</v>
@@ -96887,16 +96887,16 @@
         <v>15</v>
       </c>
       <c r="E3663" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F3663" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="G3663" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3663">
-        <v>0</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="3664" spans="1:8">
@@ -96910,13 +96910,13 @@
         <v>15</v>
       </c>
       <c r="E3664" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F3664" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="G3664" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3664">
         <v>0</v>
@@ -96933,16 +96933,16 @@
         <v>15</v>
       </c>
       <c r="E3665" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F3665" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="G3665" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3665">
-        <v>0</v>
+        <v>1.8</v>
       </c>
     </row>
     <row r="3666" spans="1:8">
@@ -96956,10 +96956,10 @@
         <v>15</v>
       </c>
       <c r="E3666" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F3666" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="G3666" t="s">
         <v>690</v>
@@ -96979,10 +96979,10 @@
         <v>15</v>
       </c>
       <c r="E3667" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="F3667" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="G3667" t="s">
         <v>690</v>
@@ -97002,10 +97002,10 @@
         <v>15</v>
       </c>
       <c r="E3668" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="F3668" t="s">
-        <v>482</v>
+        <v>449</v>
       </c>
       <c r="G3668" t="s">
         <v>690</v>
@@ -97025,16 +97025,16 @@
         <v>15</v>
       </c>
       <c r="E3669" t="s">
-        <v>114</v>
+        <v>257</v>
       </c>
       <c r="F3669" t="s">
-        <v>449</v>
+        <v>592</v>
       </c>
       <c r="G3669" t="s">
         <v>690</v>
       </c>
       <c r="H3669">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3670" spans="1:8">
@@ -97048,13 +97048,13 @@
         <v>15</v>
       </c>
       <c r="E3670" t="s">
-        <v>257</v>
+        <v>148</v>
       </c>
       <c r="F3670" t="s">
-        <v>592</v>
+        <v>483</v>
       </c>
       <c r="G3670" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3670">
         <v>0</v>
@@ -97071,16 +97071,16 @@
         <v>15</v>
       </c>
       <c r="E3671" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F3671" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="G3671" t="s">
         <v>691</v>
       </c>
       <c r="H3671">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3672" spans="1:8">
@@ -97094,10 +97094,10 @@
         <v>15</v>
       </c>
       <c r="E3672" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="F3672" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="G3672" t="s">
         <v>691</v>
@@ -97117,13 +97117,13 @@
         <v>15</v>
       </c>
       <c r="E3673" t="s">
-        <v>150</v>
+        <v>239</v>
       </c>
       <c r="F3673" t="s">
-        <v>485</v>
+        <v>574</v>
       </c>
       <c r="G3673" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3673">
         <v>0</v>
@@ -97134,16 +97134,16 @@
         <v>18</v>
       </c>
       <c r="C3674">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3674" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3674" t="s">
-        <v>239</v>
+        <v>184</v>
       </c>
       <c r="F3674" t="s">
-        <v>574</v>
+        <v>519</v>
       </c>
       <c r="G3674" t="s">
         <v>690</v>
@@ -97163,10 +97163,10 @@
         <v>16</v>
       </c>
       <c r="E3675" t="s">
-        <v>184</v>
+        <v>153</v>
       </c>
       <c r="F3675" t="s">
-        <v>519</v>
+        <v>488</v>
       </c>
       <c r="G3675" t="s">
         <v>690</v>
@@ -97186,16 +97186,16 @@
         <v>16</v>
       </c>
       <c r="E3676" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F3676" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="G3676" t="s">
         <v>690</v>
       </c>
       <c r="H3676">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="3677" spans="1:8">
@@ -97209,16 +97209,16 @@
         <v>16</v>
       </c>
       <c r="E3677" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="F3677" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="G3677" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3677">
-        <v>0</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="3678" spans="1:8">
@@ -97232,10 +97232,10 @@
         <v>16</v>
       </c>
       <c r="E3678" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="F3678" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="G3678" t="s">
         <v>691</v>
@@ -97255,16 +97255,16 @@
         <v>16</v>
       </c>
       <c r="E3679" t="s">
-        <v>159</v>
+        <v>189</v>
       </c>
       <c r="F3679" t="s">
-        <v>494</v>
+        <v>524</v>
       </c>
       <c r="G3679" t="s">
         <v>691</v>
       </c>
       <c r="H3679">
-        <v>0</v>
+        <v>15.3</v>
       </c>
     </row>
     <row r="3680" spans="1:8">
@@ -97278,16 +97278,16 @@
         <v>16</v>
       </c>
       <c r="E3680" t="s">
-        <v>189</v>
+        <v>243</v>
       </c>
       <c r="F3680" t="s">
-        <v>524</v>
+        <v>578</v>
       </c>
       <c r="G3680" t="s">
         <v>691</v>
       </c>
       <c r="H3680">
-        <v>7.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3681" spans="1:8">
@@ -97301,16 +97301,16 @@
         <v>16</v>
       </c>
       <c r="E3681" t="s">
-        <v>243</v>
+        <v>160</v>
       </c>
       <c r="F3681" t="s">
-        <v>578</v>
+        <v>495</v>
       </c>
       <c r="G3681" t="s">
         <v>691</v>
       </c>
       <c r="H3681">
-        <v>0</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="3682" spans="1:8">
@@ -97324,16 +97324,16 @@
         <v>16</v>
       </c>
       <c r="E3682" t="s">
-        <v>160</v>
+        <v>334</v>
       </c>
       <c r="F3682" t="s">
-        <v>495</v>
+        <v>669</v>
       </c>
       <c r="G3682" t="s">
         <v>691</v>
       </c>
       <c r="H3682">
-        <v>2.1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="3683" spans="1:8">
@@ -97347,16 +97347,16 @@
         <v>16</v>
       </c>
       <c r="E3683" t="s">
-        <v>334</v>
+        <v>162</v>
       </c>
       <c r="F3683" t="s">
-        <v>669</v>
+        <v>497</v>
       </c>
       <c r="G3683" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3683">
-        <v>0</v>
+        <v>2.44</v>
       </c>
     </row>
     <row r="3684" spans="1:8">
@@ -97370,16 +97370,16 @@
         <v>16</v>
       </c>
       <c r="E3684" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F3684" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G3684" t="s">
         <v>690</v>
       </c>
       <c r="H3684">
-        <v>0.64</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3685" spans="1:8">
@@ -97393,16 +97393,16 @@
         <v>16</v>
       </c>
       <c r="E3685" t="s">
-        <v>163</v>
+        <v>333</v>
       </c>
       <c r="F3685" t="s">
-        <v>498</v>
+        <v>668</v>
       </c>
       <c r="G3685" t="s">
         <v>690</v>
       </c>
       <c r="H3685">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3686" spans="1:8">
@@ -97416,13 +97416,13 @@
         <v>16</v>
       </c>
       <c r="E3686" t="s">
-        <v>333</v>
+        <v>164</v>
       </c>
       <c r="F3686" t="s">
-        <v>668</v>
+        <v>499</v>
       </c>
       <c r="G3686" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3686">
         <v>0</v>
@@ -97439,10 +97439,10 @@
         <v>16</v>
       </c>
       <c r="E3687" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="F3687" t="s">
-        <v>499</v>
+        <v>532</v>
       </c>
       <c r="G3687" t="s">
         <v>691</v>
@@ -97462,13 +97462,13 @@
         <v>16</v>
       </c>
       <c r="E3688" t="s">
-        <v>197</v>
+        <v>165</v>
       </c>
       <c r="F3688" t="s">
-        <v>532</v>
+        <v>500</v>
       </c>
       <c r="G3688" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3688">
         <v>0</v>
@@ -97485,16 +97485,16 @@
         <v>16</v>
       </c>
       <c r="E3689" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F3689" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="G3689" t="s">
         <v>690</v>
       </c>
       <c r="H3689">
-        <v>0</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="3690" spans="1:8">
@@ -97508,13 +97508,13 @@
         <v>16</v>
       </c>
       <c r="E3690" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F3690" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="G3690" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3690">
         <v>0</v>
@@ -97531,16 +97531,16 @@
         <v>16</v>
       </c>
       <c r="E3691" t="s">
-        <v>167</v>
+        <v>135</v>
       </c>
       <c r="F3691" t="s">
-        <v>502</v>
+        <v>470</v>
       </c>
       <c r="G3691" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3691">
-        <v>0</v>
+        <v>0.28</v>
       </c>
     </row>
     <row r="3692" spans="1:8">
@@ -97548,16 +97548,16 @@
         <v>18</v>
       </c>
       <c r="C3692">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3692" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3692" t="s">
-        <v>135</v>
+        <v>225</v>
       </c>
       <c r="F3692" t="s">
-        <v>470</v>
+        <v>560</v>
       </c>
       <c r="G3692" t="s">
         <v>690</v>
@@ -97577,16 +97577,16 @@
         <v>17</v>
       </c>
       <c r="E3693" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="F3693" t="s">
-        <v>560</v>
+        <v>572</v>
       </c>
       <c r="G3693" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3693">
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3694" spans="1:8">
@@ -97600,10 +97600,10 @@
         <v>17</v>
       </c>
       <c r="E3694" t="s">
-        <v>237</v>
+        <v>259</v>
       </c>
       <c r="F3694" t="s">
-        <v>572</v>
+        <v>594</v>
       </c>
       <c r="G3694" t="s">
         <v>691</v>
@@ -97623,16 +97623,16 @@
         <v>17</v>
       </c>
       <c r="E3695" t="s">
-        <v>259</v>
+        <v>169</v>
       </c>
       <c r="F3695" t="s">
-        <v>594</v>
+        <v>504</v>
       </c>
       <c r="G3695" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3695">
-        <v>0</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="3696" spans="1:8">
@@ -97646,16 +97646,16 @@
         <v>17</v>
       </c>
       <c r="E3696" t="s">
-        <v>169</v>
+        <v>23</v>
       </c>
       <c r="F3696" t="s">
-        <v>504</v>
+        <v>358</v>
       </c>
       <c r="G3696" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3696">
-        <v>2.6</v>
+        <v>3.2</v>
       </c>
     </row>
     <row r="3697" spans="1:8">
@@ -97669,13 +97669,13 @@
         <v>17</v>
       </c>
       <c r="E3697" t="s">
-        <v>23</v>
+        <v>171</v>
       </c>
       <c r="F3697" t="s">
-        <v>358</v>
+        <v>506</v>
       </c>
       <c r="G3697" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3697">
         <v>0</v>
@@ -97692,10 +97692,10 @@
         <v>17</v>
       </c>
       <c r="E3698" t="s">
-        <v>171</v>
+        <v>260</v>
       </c>
       <c r="F3698" t="s">
-        <v>506</v>
+        <v>595</v>
       </c>
       <c r="G3698" t="s">
         <v>690</v>
@@ -97715,13 +97715,13 @@
         <v>17</v>
       </c>
       <c r="E3699" t="s">
-        <v>260</v>
+        <v>125</v>
       </c>
       <c r="F3699" t="s">
-        <v>595</v>
+        <v>460</v>
       </c>
       <c r="G3699" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3699">
         <v>0</v>
@@ -97738,16 +97738,16 @@
         <v>17</v>
       </c>
       <c r="E3700" t="s">
-        <v>125</v>
+        <v>261</v>
       </c>
       <c r="F3700" t="s">
-        <v>460</v>
+        <v>596</v>
       </c>
       <c r="G3700" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3700">
-        <v>0</v>
+        <v>15.6</v>
       </c>
     </row>
     <row r="3701" spans="1:8">
@@ -97761,16 +97761,16 @@
         <v>17</v>
       </c>
       <c r="E3701" t="s">
-        <v>261</v>
+        <v>172</v>
       </c>
       <c r="F3701" t="s">
-        <v>596</v>
+        <v>507</v>
       </c>
       <c r="G3701" t="s">
         <v>690</v>
       </c>
       <c r="H3701">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="3702" spans="1:8">
@@ -97784,13 +97784,13 @@
         <v>17</v>
       </c>
       <c r="E3702" t="s">
-        <v>172</v>
+        <v>316</v>
       </c>
       <c r="F3702" t="s">
-        <v>507</v>
+        <v>651</v>
       </c>
       <c r="G3702" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3702">
         <v>0</v>
@@ -97807,16 +97807,16 @@
         <v>17</v>
       </c>
       <c r="E3703" t="s">
-        <v>316</v>
+        <v>175</v>
       </c>
       <c r="F3703" t="s">
-        <v>651</v>
+        <v>510</v>
       </c>
       <c r="G3703" t="s">
         <v>691</v>
       </c>
       <c r="H3703">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3704" spans="1:8">
@@ -97830,16 +97830,16 @@
         <v>17</v>
       </c>
       <c r="E3704" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="F3704" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="G3704" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3704">
-        <v>0</v>
+        <v>26.2</v>
       </c>
     </row>
     <row r="3705" spans="1:8">
@@ -97853,16 +97853,16 @@
         <v>17</v>
       </c>
       <c r="E3705" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="F3705" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="G3705" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3705">
-        <v>12.08</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3706" spans="1:8">
@@ -97876,16 +97876,16 @@
         <v>17</v>
       </c>
       <c r="E3706" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="F3706" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="G3706" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3706">
-        <v>0</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="3707" spans="1:8">
@@ -97899,13 +97899,13 @@
         <v>17</v>
       </c>
       <c r="E3707" t="s">
-        <v>180</v>
+        <v>100</v>
       </c>
       <c r="F3707" t="s">
-        <v>515</v>
+        <v>435</v>
       </c>
       <c r="G3707" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3707">
         <v>0</v>
@@ -97922,13 +97922,13 @@
         <v>17</v>
       </c>
       <c r="E3708" t="s">
-        <v>100</v>
+        <v>181</v>
       </c>
       <c r="F3708" t="s">
-        <v>435</v>
+        <v>516</v>
       </c>
       <c r="G3708" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3708">
         <v>0</v>
@@ -97939,22 +97939,22 @@
         <v>18</v>
       </c>
       <c r="C3709">
+        <v>11</v>
+      </c>
+      <c r="D3709" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3709" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3709" t="s">
+        <v>438</v>
+      </c>
+      <c r="G3709" t="s">
+        <v>690</v>
+      </c>
+      <c r="H3709">
         <v>10</v>
-      </c>
-      <c r="D3709" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3709" t="s">
-        <v>181</v>
-      </c>
-      <c r="F3709" t="s">
-        <v>516</v>
-      </c>
-      <c r="G3709" t="s">
-        <v>690</v>
-      </c>
-      <c r="H3709">
-        <v>0</v>
       </c>
     </row>
     <row r="3710" spans="1:8">
@@ -97968,13 +97968,13 @@
         <v>18</v>
       </c>
       <c r="E3710" t="s">
-        <v>103</v>
+        <v>233</v>
       </c>
       <c r="F3710" t="s">
-        <v>438</v>
+        <v>568</v>
       </c>
       <c r="G3710" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3710">
         <v>0</v>
@@ -97991,16 +97991,16 @@
         <v>18</v>
       </c>
       <c r="E3711" t="s">
-        <v>233</v>
+        <v>58</v>
       </c>
       <c r="F3711" t="s">
-        <v>568</v>
+        <v>393</v>
       </c>
       <c r="G3711" t="s">
         <v>691</v>
       </c>
       <c r="H3711">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3712" spans="1:8">
@@ -98014,16 +98014,16 @@
         <v>18</v>
       </c>
       <c r="E3712" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="F3712" t="s">
-        <v>393</v>
+        <v>361</v>
       </c>
       <c r="G3712" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3712">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3713" spans="1:8">
@@ -98037,16 +98037,16 @@
         <v>18</v>
       </c>
       <c r="E3713" t="s">
-        <v>26</v>
+        <v>342</v>
       </c>
       <c r="F3713" t="s">
-        <v>361</v>
+        <v>677</v>
       </c>
       <c r="G3713" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3713">
-        <v>0.7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3714" spans="1:8">
@@ -98060,16 +98060,16 @@
         <v>18</v>
       </c>
       <c r="E3714" t="s">
-        <v>342</v>
+        <v>188</v>
       </c>
       <c r="F3714" t="s">
-        <v>677</v>
+        <v>523</v>
       </c>
       <c r="G3714" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3714">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="3715" spans="1:8">
@@ -98083,10 +98083,10 @@
         <v>18</v>
       </c>
       <c r="E3715" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="F3715" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="G3715" t="s">
         <v>690</v>
@@ -98106,10 +98106,10 @@
         <v>18</v>
       </c>
       <c r="E3716" t="s">
-        <v>190</v>
+        <v>262</v>
       </c>
       <c r="F3716" t="s">
-        <v>525</v>
+        <v>597</v>
       </c>
       <c r="G3716" t="s">
         <v>690</v>
@@ -98129,13 +98129,13 @@
         <v>18</v>
       </c>
       <c r="E3717" t="s">
-        <v>262</v>
+        <v>192</v>
       </c>
       <c r="F3717" t="s">
-        <v>597</v>
+        <v>527</v>
       </c>
       <c r="G3717" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3717">
         <v>0</v>
@@ -98152,10 +98152,10 @@
         <v>18</v>
       </c>
       <c r="E3718" t="s">
-        <v>192</v>
+        <v>343</v>
       </c>
       <c r="F3718" t="s">
-        <v>527</v>
+        <v>678</v>
       </c>
       <c r="G3718" t="s">
         <v>691</v>
@@ -98175,10 +98175,10 @@
         <v>18</v>
       </c>
       <c r="E3719" t="s">
-        <v>343</v>
+        <v>161</v>
       </c>
       <c r="F3719" t="s">
-        <v>678</v>
+        <v>496</v>
       </c>
       <c r="G3719" t="s">
         <v>691</v>
@@ -98198,13 +98198,13 @@
         <v>18</v>
       </c>
       <c r="E3720" t="s">
-        <v>161</v>
+        <v>337</v>
       </c>
       <c r="F3720" t="s">
-        <v>496</v>
+        <v>672</v>
       </c>
       <c r="G3720" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3720">
         <v>0</v>
@@ -98221,16 +98221,16 @@
         <v>18</v>
       </c>
       <c r="E3721" t="s">
-        <v>337</v>
+        <v>195</v>
       </c>
       <c r="F3721" t="s">
-        <v>672</v>
+        <v>530</v>
       </c>
       <c r="G3721" t="s">
         <v>690</v>
       </c>
       <c r="H3721">
-        <v>0</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="3722" spans="1:8">
@@ -98244,16 +98244,16 @@
         <v>18</v>
       </c>
       <c r="E3722" t="s">
-        <v>195</v>
+        <v>33</v>
       </c>
       <c r="F3722" t="s">
-        <v>530</v>
+        <v>368</v>
       </c>
       <c r="G3722" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3722">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3723" spans="1:8">
@@ -98267,10 +98267,10 @@
         <v>18</v>
       </c>
       <c r="E3723" t="s">
-        <v>33</v>
+        <v>198</v>
       </c>
       <c r="F3723" t="s">
-        <v>368</v>
+        <v>533</v>
       </c>
       <c r="G3723" t="s">
         <v>691</v>
@@ -98290,13 +98290,13 @@
         <v>18</v>
       </c>
       <c r="E3724" t="s">
-        <v>198</v>
+        <v>216</v>
       </c>
       <c r="F3724" t="s">
-        <v>533</v>
+        <v>551</v>
       </c>
       <c r="G3724" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3724">
         <v>0</v>
@@ -98313,16 +98313,16 @@
         <v>18</v>
       </c>
       <c r="E3725" t="s">
-        <v>216</v>
+        <v>296</v>
       </c>
       <c r="F3725" t="s">
-        <v>551</v>
+        <v>631</v>
       </c>
       <c r="G3725" t="s">
         <v>690</v>
       </c>
       <c r="H3725">
-        <v>0</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="3726" spans="1:8">
@@ -98330,19 +98330,19 @@
         <v>18</v>
       </c>
       <c r="C3726">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3726" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E3726" t="s">
-        <v>296</v>
+        <v>201</v>
       </c>
       <c r="F3726" t="s">
-        <v>631</v>
+        <v>536</v>
       </c>
       <c r="G3726" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3726">
         <v>0</v>
@@ -98359,13 +98359,13 @@
         <v>19</v>
       </c>
       <c r="E3727" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="F3727" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="G3727" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3727">
         <v>0</v>
@@ -98382,16 +98382,16 @@
         <v>19</v>
       </c>
       <c r="E3728" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="F3728" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="G3728" t="s">
         <v>690</v>
       </c>
       <c r="H3728">
-        <v>0</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="3729" spans="1:8">
@@ -98405,13 +98405,13 @@
         <v>19</v>
       </c>
       <c r="E3729" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F3729" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="G3729" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3729">
         <v>0</v>
@@ -98428,13 +98428,13 @@
         <v>19</v>
       </c>
       <c r="E3730" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="F3730" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="G3730" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3730">
         <v>0</v>
@@ -98451,10 +98451,10 @@
         <v>19</v>
       </c>
       <c r="E3731" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F3731" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="G3731" t="s">
         <v>690</v>
@@ -98474,16 +98474,16 @@
         <v>19</v>
       </c>
       <c r="E3732" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F3732" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="G3732" t="s">
         <v>690</v>
       </c>
       <c r="H3732">
-        <v>0</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="3733" spans="1:8">
@@ -98497,10 +98497,10 @@
         <v>19</v>
       </c>
       <c r="E3733" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="F3733" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="G3733" t="s">
         <v>690</v>
@@ -98520,10 +98520,10 @@
         <v>19</v>
       </c>
       <c r="E3734" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F3734" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="G3734" t="s">
         <v>690</v>
@@ -98543,10 +98543,10 @@
         <v>19</v>
       </c>
       <c r="E3735" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F3735" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="G3735" t="s">
         <v>690</v>
@@ -98566,13 +98566,13 @@
         <v>19</v>
       </c>
       <c r="E3736" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F3736" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="G3736" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="H3736">
         <v>0</v>
@@ -98589,10 +98589,10 @@
         <v>19</v>
       </c>
       <c r="E3737" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F3737" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="G3737" t="s">
         <v>691</v>
@@ -98612,10 +98612,10 @@
         <v>19</v>
       </c>
       <c r="E3738" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F3738" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="G3738" t="s">
         <v>691</v>
@@ -98635,10 +98635,10 @@
         <v>19</v>
       </c>
       <c r="E3739" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="F3739" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="G3739" t="s">
         <v>691</v>
@@ -98658,10 +98658,10 @@
         <v>19</v>
       </c>
       <c r="E3740" t="s">
-        <v>217</v>
+        <v>320</v>
       </c>
       <c r="F3740" t="s">
-        <v>552</v>
+        <v>655</v>
       </c>
       <c r="G3740" t="s">
         <v>691</v>
@@ -98681,39 +98681,16 @@
         <v>19</v>
       </c>
       <c r="E3741" t="s">
-        <v>320</v>
+        <v>183</v>
       </c>
       <c r="F3741" t="s">
-        <v>655</v>
+        <v>518</v>
       </c>
       <c r="G3741" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="H3741">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3742" spans="1:8">
-      <c r="A3742">
-        <v>18</v>
-      </c>
-      <c r="C3742">
-        <v>12</v>
-      </c>
-      <c r="D3742" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3742" t="s">
-        <v>183</v>
-      </c>
-      <c r="F3742" t="s">
-        <v>518</v>
-      </c>
-      <c r="G3742" t="s">
-        <v>690</v>
-      </c>
-      <c r="H3742">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>